<commit_message>
[ADD] project field in excel asset report
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_asset.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_asset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">ขื่อบริษัท</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">เอกสารอ้างอิง</t>
+  </si>
+  <si>
+    <t xml:space="preserve">โปรเจค</t>
   </si>
   <si>
     <t xml:space="preserve">หมายเหตุ</t>
@@ -309,10 +312,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,9 +327,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="13" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="20" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +356,8 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -371,7 +377,8 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="4"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -391,7 +398,8 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="4"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4"/>
@@ -452,7 +460,10 @@
       <c r="O6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="P6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -463,14 +474,14 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="6"/>
@@ -478,13 +489,14 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="S7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="T7" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
+  <mergeCells count="20">
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="A4:P4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -500,7 +512,8 @@
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="T6:T7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>